<commit_message>
legacy data and official division for people
</commit_message>
<xml_diff>
--- a/database/_legacy-data/fixtures.xlsx
+++ b/database/_legacy-data/fixtures.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="17970" windowHeight="12555" xr2:uid="{8455CC45-3136-47B0-AF7C-E27F4836AC35}"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="17970" windowHeight="12555" xr2:uid="{8455CC45-3136-47B0-AF7C-E27F4836AC35}"/>
   </bookViews>
   <sheets>
     <sheet name="2017 - 1 " sheetId="1" r:id="rId1"/>
@@ -144,6 +144,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -175,7 +178,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -492,15 +495,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6754C2F-3520-4F81-9DD6-817784A1132E}">
   <dimension ref="A1:T134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B7:B8"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
@@ -1496,6 +1499,7 @@
       <c r="B28">
         <v>363</v>
       </c>
+      <c r="C28" s="1"/>
       <c r="D28">
         <v>22</v>
       </c>
@@ -4910,5 +4914,6 @@
   </sheetData>
   <autoFilter ref="A1:T134" xr:uid="{7251E6BB-0FD6-4145-873A-2A609487CDEA}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>